<commit_message>
new subset to include Case Status
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Search_Results/artifacts/service_model/information_model/IEPD/documentation/Court_Case_Search_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Search_Results/artifacts/service_model/information_model/IEPD/documentation/Court_Case_Search_Results-Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
+    <workbookView xWindow="29800" yWindow="-1000" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Query Request Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
   <si>
     <t>CLASS</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>partyID</t>
+  </si>
+  <si>
+    <t>Case Status</t>
+  </si>
+  <si>
+    <t>/exch:CourtCaseSearchResults/nc:Case/nc:ActivityStatus/nc:StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>status of a case</t>
   </si>
 </sst>
 </file>
@@ -1009,13 +1018,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1925,11 +1934,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1960,13 +1969,13 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="28">
       <c r="A3" s="5"/>
@@ -2038,308 +2047,321 @@
     <row r="8" spans="1:6">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2"/>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2"/>
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:6" ht="28">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="8" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="9"/>
-      <c r="B12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="9"/>
+      <c r="B13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="30">
-      <c r="A14"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="30">
+      <c r="A15"/>
+      <c r="B15" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D14"/>
-      <c r="E14" s="10" t="s">
+      <c r="D15"/>
+      <c r="E15" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="28">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="42">
+    <row r="21" spans="1:5">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="42">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="30">
-      <c r="B25" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="C25" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>75</v>
+        <v>59</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30">
       <c r="B26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30">
+      <c r="B27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C33" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new subset to include Case Status and update subset
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Search_Results/artifacts/service_model/information_model/IEPD/documentation/Court_Case_Search_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Search_Results/artifacts/service_model/information_model/IEPD/documentation/Court_Case_Search_Results-Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
+    <workbookView xWindow="29800" yWindow="-1000" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Query Request Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
   <si>
     <t>CLASS</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>partyID</t>
+  </si>
+  <si>
+    <t>Case Status</t>
+  </si>
+  <si>
+    <t>/exch:CourtCaseSearchResults/nc:Case/nc:ActivityStatus/nc:StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>status of a case</t>
   </si>
 </sst>
 </file>
@@ -1009,13 +1018,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1925,11 +1934,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1960,13 +1969,13 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="28">
       <c r="A3" s="5"/>
@@ -2038,308 +2047,321 @@
     <row r="8" spans="1:6">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2"/>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2"/>
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:6" ht="28">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="8" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="9"/>
-      <c r="B12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="9"/>
+      <c r="B13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="30">
-      <c r="A14"/>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="30">
+      <c r="A15"/>
+      <c r="B15" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D14"/>
-      <c r="E14" s="10" t="s">
+      <c r="D15"/>
+      <c r="E15" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="28">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="42">
+    <row r="21" spans="1:5">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="42">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="30">
-      <c r="B25" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="C25" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>75</v>
+        <v>59</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30">
       <c r="B26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30">
+      <c r="B27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C33" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>